<commit_message>
Mise à jour de l'avancement
</commit_message>
<xml_diff>
--- a/doc/checkCdC_89.xlsx
+++ b/doc/checkCdC_89.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="77">
   <si>
     <t xml:space="preserve">Master Bioinformatique – Université de Rouen Normandie - M2.1 Semestre 3</t>
   </si>
@@ -184,6 +184,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">PARTIELLEMENT</t>
+  </si>
+  <si>
     <t xml:space="preserve">J</t>
   </si>
   <si>
@@ -222,13 +225,19 @@
     <t xml:space="preserve">GO terms : quelle banque; SEA +GSEA; quel test statistique ? Avez-vous traité le choix du nivo des GoTerms ( multi-level ?)</t>
   </si>
   <si>
+    <t xml:space="preserve">le choix du nivo des GoTerms ( multi-level ?)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pathways : quelle banque; SEA+GSEA quel test statistique ?</t>
   </si>
   <si>
+    <t xml:space="preserve">SEA+GSEA quel test statistique ?</t>
+  </si>
+  <si>
     <t xml:space="preserve">Domains: quelle banque; codage "maison" en SEA uniquement</t>
   </si>
   <si>
-    <t xml:space="preserve">EN CONTINUE</t>
+    <t xml:space="preserve">EN CONTINU</t>
   </si>
   <si>
     <r>
@@ -332,18 +341,30 @@
     <t xml:space="preserve"> ergonomie/ choix et justification de la disposition des cadres</t>
   </si>
   <si>
+    <t xml:space="preserve">ergonomie</t>
+  </si>
+  <si>
     <t xml:space="preserve">S</t>
   </si>
   <si>
     <t xml:space="preserve">input, traitement du format et les paramètres de lancement ( seuil, niveau GO, catégories GO) </t>
   </si>
   <si>
+    <t xml:space="preserve"> paramètres de lancement </t>
+  </si>
+  <si>
     <t xml:space="preserve">Input : doit comporter une précision de l'origine du gene ID ( NCBI, Ensembl)</t>
   </si>
   <si>
+    <t xml:space="preserve">OUI</t>
+  </si>
+  <si>
     <t xml:space="preserve">Input : doit comporter un paramètre de choix de l'espace (BiomaRt)</t>
   </si>
   <si>
+    <t xml:space="preserve">paramètre de choix</t>
+  </si>
+  <si>
     <t xml:space="preserve">Quatre onglets dans le menu : whole data inspection; GO terms enrichement; Pathway enrichment; Protein Domain enrichement</t>
   </si>
   <si>
@@ -380,6 +401,9 @@
     <t xml:space="preserve">Autres packages pour quelles fonctionnalités ? BiomaRt pour connexion à Ensembl; autre pour import du background, plot de graphe</t>
   </si>
   <si>
+    <t xml:space="preserve">Autres packages pour quelles fonctionnalités ? </t>
+  </si>
+  <si>
     <t xml:space="preserve">fonctions R utilisées pour quelles fonctionnalités ?</t>
   </si>
   <si>
@@ -389,6 +413,12 @@
     <t xml:space="preserve">Comment gérez-vous la reconnaissance du format input ?</t>
   </si>
   <si>
+    <t xml:space="preserve">Vérification du format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X/J</t>
+  </si>
+  <si>
     <t xml:space="preserve">00101010</t>
   </si>
   <si>
@@ -404,22 +434,19 @@
     <t xml:space="preserve">Il est recommandé d'utiliser un outil de suivi de version </t>
   </si>
   <si>
-    <t xml:space="preserve">OUI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">framagit</t>
+    <t xml:space="preserve">GitHub</t>
   </si>
   <si>
     <t xml:space="preserve">Comment le travail se répartit-il dans l'équipe ?</t>
   </si>
   <si>
-    <t xml:space="preserve">S : interface / X : packages / J : doc / H : graphes</t>
+    <t xml:space="preserve">S : interface / X : packages / J : doc  + GSEA / H : graphes + SEA</t>
   </si>
   <si>
     <t xml:space="preserve">La documentation technique et utilisateur</t>
   </si>
   <si>
-    <t xml:space="preserve">Avez-vous réalisé un read me, neautamman pour les versions et les dépendances ?</t>
+    <t xml:space="preserve">Avez-vous réalisé un read me, notamment pour les versions et les dépendances ?</t>
   </si>
   <si>
     <t xml:space="preserve">Le schéma général de la solution est-il complet ? Noms des packages, fonction des packages, fichier input, fichier output, ressources banques externes</t>
@@ -537,7 +564,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -566,6 +593,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF6666"/>
         <bgColor rgb="FFED7D31"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -622,7 +655,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -703,6 +736,10 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -719,6 +756,10 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -735,11 +776,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -822,16 +859,16 @@
   </sheetPr>
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="59.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="65.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="41.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="11.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="54.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="11.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="32.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="10.53"/>
   </cols>
@@ -947,131 +984,135 @@
       <c r="A13" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="20"/>
+      <c r="B13" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="21"/>
       <c r="D13" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E13" s="13"/>
     </row>
     <row r="14" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="18"/>
       <c r="D14" s="18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="22"/>
+        <v>22</v>
+      </c>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23"/>
       <c r="D15" s="18"/>
       <c r="E15" s="13"/>
     </row>
-    <row r="16" customFormat="false" ht="24.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="21"/>
+    <row r="16" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>24</v>
+      </c>
       <c r="D16" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="13"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="13"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="21"/>
+      <c r="C17" s="24" t="s">
+        <v>26</v>
+      </c>
       <c r="D17" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E17" s="13"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="23" t="s">
-        <v>24</v>
+      <c r="A18" s="24" t="s">
+        <v>27</v>
       </c>
       <c r="B18" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="21"/>
+      <c r="C18" s="22"/>
       <c r="D18" s="18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="34.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="15" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="22"/>
+      <c r="C19" s="23"/>
       <c r="D19" s="18"/>
       <c r="E19" s="13"/>
     </row>
     <row r="20" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="15" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="21"/>
+      <c r="C20" s="22"/>
       <c r="D20" s="18"/>
       <c r="E20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="15" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="21"/>
+      <c r="C21" s="22"/>
       <c r="D21" s="18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="24.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="15" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="21"/>
+      <c r="C22" s="22"/>
       <c r="D22" s="18"/>
       <c r="E22" s="13"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="12" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
@@ -1079,158 +1120,164 @@
       <c r="E23" s="13"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="21"/>
+      <c r="A24" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>36</v>
+      </c>
       <c r="D24" s="18" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E24" s="13" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="24.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="21"/>
+    <row r="25" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>39</v>
+      </c>
       <c r="D25" s="18" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E25" s="13" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="24.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="21"/>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="22"/>
       <c r="D26" s="18" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E26" s="13" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="21"/>
+      <c r="A27" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>43</v>
+      </c>
       <c r="D27" s="18" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E27" s="13" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="23" t="s">
+    <row r="28" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="22"/>
+      <c r="D28" s="18" t="s">
         <v>37</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="21"/>
-      <c r="D28" s="18" t="s">
-        <v>33</v>
       </c>
       <c r="E28" s="13" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" s="21"/>
+    <row r="29" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="22"/>
       <c r="D29" s="18" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E29" s="13" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="23" t="s">
-        <v>39</v>
+      <c r="A30" s="24" t="s">
+        <v>46</v>
       </c>
       <c r="B30" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="21"/>
+      <c r="C30" s="22"/>
       <c r="D30" s="18" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E30" s="13" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="29.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="23" t="s">
-        <v>40</v>
+      <c r="A31" s="24" t="s">
+        <v>47</v>
       </c>
       <c r="B31" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="21"/>
+      <c r="C31" s="22"/>
       <c r="D31" s="18" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E31" s="13" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="25.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="23" t="s">
-        <v>41</v>
+      <c r="A32" s="24" t="s">
+        <v>48</v>
       </c>
       <c r="B32" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="21"/>
+      <c r="C32" s="22"/>
       <c r="D32" s="18" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E32" s="13" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="23" t="s">
-        <v>42</v>
+      <c r="A33" s="24" t="s">
+        <v>49</v>
       </c>
       <c r="B33" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="21"/>
+      <c r="C33" s="22"/>
       <c r="D33" s="18" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E33" s="13" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="24" t="s">
-        <v>43</v>
+      <c r="A34" s="26" t="s">
+        <v>50</v>
       </c>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
@@ -1238,121 +1285,127 @@
       <c r="E34" s="13"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="25" t="s">
-        <v>44</v>
+      <c r="A35" s="27" t="s">
+        <v>51</v>
       </c>
       <c r="B35" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="21"/>
+      <c r="C35" s="22"/>
       <c r="D35" s="18" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="E35" s="13"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="26" t="s">
-        <v>46</v>
+      <c r="A36" s="28" t="s">
+        <v>53</v>
       </c>
       <c r="B36" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C36" s="21"/>
+      <c r="C36" s="22"/>
       <c r="D36" s="18"/>
       <c r="E36" s="13" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="26" t="s">
-        <v>47</v>
+      <c r="A37" s="28" t="s">
+        <v>54</v>
       </c>
       <c r="B37" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="21"/>
+      <c r="C37" s="22"/>
       <c r="D37" s="18"/>
       <c r="E37" s="13" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="40.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="B38" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" s="21"/>
+      <c r="A38" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>56</v>
+      </c>
       <c r="D38" s="18"/>
       <c r="E38" s="13" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="26" t="s">
-        <v>49</v>
+      <c r="A39" s="28" t="s">
+        <v>57</v>
       </c>
       <c r="B39" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="21"/>
+      <c r="C39" s="22"/>
       <c r="D39" s="18"/>
       <c r="E39" s="13"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="B40" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C40" s="21"/>
+      <c r="A40" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="22"/>
       <c r="D40" s="18"/>
       <c r="E40" s="13"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="B41" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="27" t="s">
-        <v>52</v>
+      <c r="A41" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E41" s="29" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="25" t="s">
-        <v>53</v>
+      <c r="A42" s="27" t="s">
+        <v>63</v>
       </c>
       <c r="B42" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="21"/>
+      <c r="C42" s="22"/>
       <c r="D42" s="18"/>
-      <c r="E42" s="27" t="s">
-        <v>52</v>
+      <c r="E42" s="29" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="25" t="s">
-        <v>54</v>
+      <c r="A43" s="27" t="s">
+        <v>64</v>
       </c>
       <c r="B43" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C43" s="21"/>
+      <c r="C43" s="22"/>
       <c r="D43" s="18"/>
-      <c r="E43" s="27" t="s">
-        <v>52</v>
+      <c r="E43" s="29" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="24" t="s">
-        <v>55</v>
+      <c r="A44" s="26" t="s">
+        <v>65</v>
       </c>
       <c r="B44" s="13"/>
       <c r="C44" s="13"/>
@@ -1360,115 +1413,115 @@
       <c r="E44" s="13"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="B45" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="C45" s="21" t="s">
-        <v>58</v>
+      <c r="A45" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C45" s="22" t="s">
+        <v>67</v>
       </c>
       <c r="D45" s="18"/>
       <c r="E45" s="13"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="B46" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="C46" s="21" t="s">
-        <v>60</v>
+      <c r="A46" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B46" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C46" s="22" t="s">
+        <v>69</v>
       </c>
       <c r="D46" s="18"/>
       <c r="E46" s="13"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="24" t="s">
-        <v>61</v>
+      <c r="A47" s="26" t="s">
+        <v>70</v>
       </c>
       <c r="B47" s="13"/>
       <c r="C47" s="13"/>
       <c r="D47" s="14"/>
       <c r="E47" s="13"/>
     </row>
-    <row r="48" customFormat="false" ht="24.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="B48" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C48" s="21"/>
+    <row r="48" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B48" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48" s="22"/>
       <c r="D48" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E48" s="13"/>
     </row>
     <row r="49" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="23" t="s">
-        <v>63</v>
+      <c r="A49" s="24" t="s">
+        <v>72</v>
       </c>
       <c r="B49" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C49" s="21"/>
+      <c r="C49" s="22"/>
       <c r="D49" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E49" s="13"/>
     </row>
     <row r="50" customFormat="false" ht="24.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="29" t="s">
-        <v>64</v>
+      <c r="A50" s="30" t="s">
+        <v>73</v>
       </c>
       <c r="B50" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C50" s="21"/>
+      <c r="C50" s="22"/>
       <c r="D50" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E50" s="13"/>
     </row>
     <row r="51" customFormat="false" ht="24.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="29" t="s">
-        <v>65</v>
+      <c r="A51" s="30" t="s">
+        <v>74</v>
       </c>
       <c r="B51" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C51" s="21"/>
+      <c r="C51" s="22"/>
       <c r="D51" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E51" s="13"/>
     </row>
     <row r="52" customFormat="false" ht="24.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="29" t="s">
-        <v>66</v>
+      <c r="A52" s="30" t="s">
+        <v>75</v>
       </c>
       <c r="B52" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C52" s="21"/>
+      <c r="C52" s="22"/>
       <c r="D52" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E52" s="13"/>
     </row>
     <row r="53" customFormat="false" ht="24.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="29" t="s">
-        <v>67</v>
+      <c r="A53" s="30" t="s">
+        <v>76</v>
       </c>
       <c r="B53" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C53" s="21"/>
+      <c r="C53" s="22"/>
       <c r="D53" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E53" s="13"/>
     </row>

</xml_diff>

<commit_message>
Mise à jour de l'attribution des tâches
</commit_message>
<xml_diff>
--- a/doc/checkCdC_89.xlsx
+++ b/doc/checkCdC_89.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="79">
   <si>
     <t xml:space="preserve">Master Bioinformatique – Université de Rouen Normandie - M2.1 Semestre 3</t>
   </si>
@@ -263,6 +263,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">X/S</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b val="true"/>
@@ -453,6 +456,9 @@
   </si>
   <si>
     <t xml:space="preserve">La documentation utilisateur inclut-elle les explications fondamentales des modèles SEA et GSEA (avec bibliographie)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H/J</t>
   </si>
   <si>
     <t xml:space="preserve">La documentation utilisateur ( ou tutoriel)  inclut-elle les explications fondamentales sur la problématique de génomes peu ou mal annotés ?</t>
@@ -859,8 +865,8 @@
   </sheetPr>
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1070,23 +1076,27 @@
         <v>14</v>
       </c>
       <c r="C19" s="23"/>
-      <c r="D19" s="18"/>
+      <c r="D19" s="18" t="s">
+        <v>30</v>
+      </c>
       <c r="E19" s="13"/>
     </row>
     <row r="20" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>14</v>
       </c>
       <c r="C20" s="22"/>
-      <c r="D20" s="18"/>
+      <c r="D20" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="E20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>14</v>
@@ -1096,23 +1106,25 @@
         <v>20</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="24.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>14</v>
       </c>
       <c r="C22" s="22"/>
-      <c r="D22" s="18"/>
+      <c r="D22" s="18" t="s">
+        <v>20</v>
+      </c>
       <c r="E22" s="13"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
@@ -1121,16 +1133,16 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="24" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B24" s="20" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E24" s="13" t="n">
         <v>2</v>
@@ -1138,16 +1150,16 @@
     </row>
     <row r="25" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B25" s="20" t="s">
         <v>17</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E25" s="13" t="n">
         <v>2</v>
@@ -1155,14 +1167,14 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="24" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C26" s="22"/>
       <c r="D26" s="18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E26" s="13" t="n">
         <v>2</v>
@@ -1170,16 +1182,16 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="24" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B27" s="20" t="s">
         <v>17</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E27" s="13" t="n">
         <v>2</v>
@@ -1187,14 +1199,14 @@
     </row>
     <row r="28" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="24" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C28" s="22"/>
       <c r="D28" s="18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E28" s="13" t="n">
         <v>2</v>
@@ -1202,14 +1214,14 @@
     </row>
     <row r="29" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="24" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C29" s="22"/>
       <c r="D29" s="18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E29" s="13" t="n">
         <v>2</v>
@@ -1217,14 +1229,14 @@
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="24" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B30" s="16" t="s">
         <v>14</v>
       </c>
       <c r="C30" s="22"/>
       <c r="D30" s="18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E30" s="13" t="n">
         <v>2</v>
@@ -1232,14 +1244,14 @@
     </row>
     <row r="31" customFormat="false" ht="29.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="24" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B31" s="16" t="s">
         <v>14</v>
       </c>
       <c r="C31" s="22"/>
       <c r="D31" s="18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E31" s="13" t="n">
         <v>2</v>
@@ -1247,14 +1259,14 @@
     </row>
     <row r="32" customFormat="false" ht="25.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="24" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B32" s="16" t="s">
         <v>14</v>
       </c>
       <c r="C32" s="22"/>
       <c r="D32" s="18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E32" s="13" t="n">
         <v>2</v>
@@ -1262,14 +1274,14 @@
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="24" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B33" s="16" t="s">
         <v>14</v>
       </c>
       <c r="C33" s="22"/>
       <c r="D33" s="18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E33" s="13" t="n">
         <v>2</v>
@@ -1277,7 +1289,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="26" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
@@ -1286,20 +1298,20 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="27" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B35" s="16" t="s">
         <v>14</v>
       </c>
       <c r="C35" s="22"/>
       <c r="D35" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E35" s="13"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="28" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B36" s="16" t="s">
         <v>14</v>
@@ -1312,7 +1324,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="28" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B37" s="16" t="s">
         <v>14</v>
@@ -1323,15 +1335,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="40.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="31.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B38" s="20" t="s">
         <v>17</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D38" s="18"/>
       <c r="E38" s="13" t="n">
@@ -1340,7 +1352,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="28" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B39" s="16" t="s">
         <v>14</v>
@@ -1351,7 +1363,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="28" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B40" s="20" t="s">
         <v>17</v>
@@ -1362,37 +1374,39 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="28" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B41" s="20" t="s">
         <v>17</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E41" s="29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="22"/>
+      <c r="D42" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E42" s="29" t="s">
         <v>63</v>
-      </c>
-      <c r="B42" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C42" s="22"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="29" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="27" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B43" s="16" t="s">
         <v>14</v>
@@ -1400,12 +1414,12 @@
       <c r="C43" s="22"/>
       <c r="D43" s="18"/>
       <c r="E43" s="29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="26" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B44" s="13"/>
       <c r="C44" s="13"/>
@@ -1414,33 +1428,33 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="24" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D45" s="18"/>
       <c r="E45" s="13"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D46" s="18"/>
       <c r="E46" s="13"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="26" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B47" s="13"/>
       <c r="C47" s="13"/>
@@ -1449,20 +1463,20 @@
     </row>
     <row r="48" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="24" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B48" s="20" t="s">
         <v>17</v>
       </c>
       <c r="C48" s="22"/>
       <c r="D48" s="18" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="E48" s="13"/>
     </row>
     <row r="49" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="24" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B49" s="16" t="s">
         <v>14</v>
@@ -1475,20 +1489,20 @@
     </row>
     <row r="50" customFormat="false" ht="24.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="30" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B50" s="16" t="s">
         <v>14</v>
       </c>
       <c r="C50" s="22"/>
       <c r="D50" s="18" t="s">
-        <v>18</v>
+        <v>75</v>
       </c>
       <c r="E50" s="13"/>
     </row>
     <row r="51" customFormat="false" ht="24.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B51" s="16" t="s">
         <v>14</v>
@@ -1501,7 +1515,7 @@
     </row>
     <row r="52" customFormat="false" ht="24.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="30" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B52" s="16" t="s">
         <v>14</v>
@@ -1514,7 +1528,7 @@
     </row>
     <row r="53" customFormat="false" ht="24.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B53" s="16" t="s">
         <v>14</v>

</xml_diff>